<commit_message>
feat(release): finalize PCB design and setup firmware environment
Hardware (Altium Designer):
- Finalized PCB layout v1.0: added 3d model for conector j2 and j3, verified Design Rules (DRC).
- Generated manufacturing artifacts: Gerber files and NC Drill data.
- Completed procurement BOM (.xlsx) according to the corporate template (including external NTC probe).
- Project structure reorganized (`Docs`, `LIB`) and ready for mentor review.

Firmware (VS Code):
- Fully configured build system for Cosmic compiler (tasks.json with cmd.exe).
- Configured automated flashing task via STVP CLI (ST-Link V2).
- Initialized firmware project structure (Core/Drivers) and verified successful compilation/flashing on hardware.
</commit_message>
<xml_diff>
--- a/Docs/Thermostat_STM8_BOM_Ajax.xlsx
+++ b/Docs/Thermostat_STM8_BOM_Ajax.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Thermostat_Tkach\Altium\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\Thermostat_Tkach\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF892DA-A90E-48D9-A9DE-5555EC18EBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BE8376-D4BB-40E3-9516-502C81EFC76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{388A08E4-6A9E-4805-A83A-142F765F91E8}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="169">
   <si>
     <t>Internal reference</t>
   </si>
@@ -523,6 +523,24 @@
   </si>
   <si>
     <t>KL-3641G-BSG</t>
+  </si>
+  <si>
+    <t>Sensor_1</t>
+  </si>
+  <si>
+    <t>NTC-10K-3950-XH2.54</t>
+  </si>
+  <si>
+    <t>Thermistor</t>
+  </si>
+  <si>
+    <t>Probe</t>
+  </si>
+  <si>
+    <t>NTC Probe Thermistor</t>
+  </si>
+  <si>
+    <t>Waterproof NTC Thermistor 10k 3950 w/ connector XH2.54</t>
   </si>
 </sst>
 </file>
@@ -708,9 +726,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -727,16 +755,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
@@ -1051,10 +1070,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB151DE5-E882-48B4-957B-28A6E3C6B74A}">
-  <dimension ref="A2:N32"/>
+  <dimension ref="A2:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1095,88 +1114,88 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="8" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="9" t="s">
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M8" s="10"/>
-      <c r="N8" s="11"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="15"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="9" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="12" t="s">
+      <c r="M9" s="15"/>
+      <c r="N9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="13" t="s">
+      <c r="G10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="13" t="s">
+      <c r="H10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="M10" s="15" t="s">
+      <c r="M10" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N10" s="12" t="s">
+      <c r="N10" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1884,6 +1903,41 @@
         <v>160</v>
       </c>
       <c r="N32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>163</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>164</v>
+      </c>
+      <c r="D33" t="s">
+        <v>107</v>
+      </c>
+      <c r="E33" s="16">
+        <v>0.01</v>
+      </c>
+      <c r="G33" t="s">
+        <v>165</v>
+      </c>
+      <c r="H33" t="s">
+        <v>166</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>167</v>
+      </c>
+      <c r="K33" t="s">
+        <v>168</v>
+      </c>
+      <c r="N33" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>